<commit_message>
last commit before branching
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devra\Documents\Shakti Files\Projects\Scraping Stock Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3075CF27-4091-4502-A790-D74E63679E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD3D45-700E-4BF5-B638-C78001306047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,27 +56,30 @@
     <t>MER</t>
   </si>
   <si>
+    <t>Current_Price</t>
+  </si>
+  <si>
+    <t>Expected_Price</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>Div_Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend </t>
+  </si>
+  <si>
+    <t>Dividend_Income</t>
+  </si>
+  <si>
+    <t>Potential_Return</t>
+  </si>
+  <si>
     <t>Growth</t>
   </si>
   <si>
-    <t>Current_Price</t>
-  </si>
-  <si>
-    <t>Expected_Price</t>
-  </si>
-  <si>
-    <t>Shares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividend </t>
-  </si>
-  <si>
-    <t>Dividend_Income</t>
-  </si>
-  <si>
-    <t>Potential_Return</t>
-  </si>
-  <si>
     <t>BMO</t>
   </si>
   <si>
@@ -92,6 +95,15 @@
     <t>Y</t>
   </si>
   <si>
+    <t>ZEB</t>
+  </si>
+  <si>
+    <t>ETF</t>
+  </si>
+  <si>
+    <t>Candian BankS</t>
+  </si>
+  <si>
     <t>Canadian Western Bank</t>
   </si>
   <si>
@@ -122,9 +134,6 @@
     <t>VEE</t>
   </si>
   <si>
-    <t>ETF</t>
-  </si>
-  <si>
     <t>World - Emerging</t>
   </si>
   <si>
@@ -143,6 +152,21 @@
     <t>RY</t>
   </si>
   <si>
+    <t>Enbridge</t>
+  </si>
+  <si>
+    <t>ENB</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>National Bank</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Netflix</t>
   </si>
   <si>
@@ -155,19 +179,19 @@
     <t>Entertainment</t>
   </si>
   <si>
-    <t>Enbridge</t>
-  </si>
-  <si>
-    <t>ENB</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>National Bank</t>
-  </si>
-  <si>
-    <t>NA</t>
+    <t>XUU</t>
+  </si>
+  <si>
+    <t>US S&amp;P</t>
+  </si>
+  <si>
+    <t>ZCN.TO</t>
+  </si>
+  <si>
+    <t>ZCN</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
   <si>
     <t>Microsoft</t>
@@ -179,46 +203,22 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>XUU</t>
-  </si>
-  <si>
-    <t>US S&amp;P</t>
-  </si>
-  <si>
-    <t>ZCN.TO</t>
-  </si>
-  <si>
-    <t>ZCN</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>XEQT</t>
   </si>
   <si>
     <t>World</t>
   </si>
   <si>
+    <t>Constellation Software</t>
+  </si>
+  <si>
+    <t>CSU</t>
+  </si>
+  <si>
     <t>Loblaw</t>
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>Constellation Software</t>
-  </si>
-  <si>
-    <t>CSU</t>
-  </si>
-  <si>
-    <t>ZEB</t>
-  </si>
-  <si>
-    <t>Candian BankS</t>
-  </si>
-  <si>
-    <t>Div_Frequency</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +629,8 @@
     <col min="14" max="14" width="19.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="8.88671875" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="22" width="8.88671875" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -656,16 +656,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>11</v>
@@ -677,24 +677,24 @@
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <v>1000</v>
@@ -721,24 +721,24 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1">
         <v>1000</v>
@@ -765,24 +765,24 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1">
         <v>1000</v>
@@ -809,24 +809,24 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1">
         <v>1000</v>
@@ -853,24 +853,24 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
         <v>1000</v>
@@ -899,19 +899,19 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1">
         <v>1000</v>
@@ -943,19 +943,19 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1">
         <v>1000</v>
@@ -984,19 +984,19 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1">
         <v>1000</v>
@@ -1025,19 +1025,19 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1">
         <v>1000</v>
@@ -1066,19 +1066,19 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F11" s="1">
         <v>1000</v>
@@ -1107,19 +1107,19 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1">
         <v>1000</v>
@@ -1148,19 +1148,19 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1">
         <v>1000</v>
@@ -1195,10 +1195,10 @@
         <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>49</v>
@@ -1231,7 +1231,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1242,10 +1242,10 @@
         <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>52</v>
@@ -1280,19 +1280,19 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1">
         <v>1000</v>
@@ -1319,24 +1319,24 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F17" s="1">
         <v>1000</v>
@@ -1368,19 +1368,19 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1">
         <v>1000</v>
@@ -1409,19 +1409,19 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
removed whitespaces from dataframe column headers
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devra\Documents\Shakti Files\Projects\Scraping Stock Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93DC327-F087-49DD-8AC6-4DC60BFD08AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F22C43-F2F4-44CB-84BA-C38244F15BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,8 +629,8 @@
     <col min="14" max="14" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="26" width="8.88671875" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="28" width="8.88671875" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -706,13 +706,13 @@
         <f t="shared" ref="J2:J19" si="0">ROUNDDOWN(F2/H2,0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K2"/>
+      <c r="L2"/>
       <c r="M2" s="2" t="e">
-        <f>J2*L2</f>
+        <f t="shared" ref="M2:M19" si="1">J2*L2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N2" s="2" t="e">
-        <f>(I2-H2)*J2</f>
+        <f t="shared" ref="N2:N19" si="2">(I2-H2)*J2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -745,13 +745,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K3"/>
+      <c r="L3"/>
       <c r="M3" s="2" t="e">
-        <f>J3*L3</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N3" s="2" t="e">
-        <f>(I3-H3)*J3</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -784,13 +784,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4"/>
+      <c r="L4"/>
       <c r="M4" s="2" t="e">
-        <f>J4*L4</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N4" s="2" t="e">
-        <f>(I4-H4)*J4</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -823,13 +823,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5"/>
+      <c r="L5"/>
       <c r="M5" s="2" t="e">
-        <f>J5*L5</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N5" s="2" t="e">
-        <f>(I5-H5)*J5</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -862,13 +862,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6"/>
+      <c r="L6"/>
       <c r="M6" s="2" t="e">
-        <f>J6*L6</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N6" s="2" t="e">
-        <f>(I6-H6)*J6</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -901,13 +901,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="2" t="e">
-        <f>J7*L7</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N7" s="2" t="e">
-        <f>(I7-H7)*J7</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -937,13 +937,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8"/>
+      <c r="L8"/>
       <c r="M8" s="2" t="e">
-        <f>J8*L8</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N8" s="2" t="e">
-        <f>(I8-H8)*J8</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -973,13 +973,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9"/>
+      <c r="L9"/>
       <c r="M9" s="2" t="e">
-        <f>J9*L9</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N9" s="2" t="e">
-        <f>(I9-H9)*J9</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1009,13 +1009,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10"/>
+      <c r="L10"/>
       <c r="M10" s="2" t="e">
-        <f>J10*L10</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N10" s="2" t="e">
-        <f>(I10-H10)*J10</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1045,13 +1045,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11"/>
+      <c r="L11"/>
       <c r="M11" s="2" t="e">
-        <f>J11*L11</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="2" t="e">
-        <f>(I11-H11)*J11</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1081,13 +1081,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12"/>
+      <c r="L12"/>
       <c r="M12" s="2" t="e">
-        <f>J12*L12</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="2" t="e">
-        <f>(I12-H12)*J12</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1117,13 +1117,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13"/>
+      <c r="L13"/>
       <c r="M13" s="2" t="e">
-        <f>J13*L13</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N13" s="2" t="e">
-        <f>(I13-H13)*J13</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1156,13 +1156,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14"/>
+      <c r="L14"/>
       <c r="M14" s="2" t="e">
-        <f>J14*L14</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="2" t="e">
-        <f>(I14-H14)*J14</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O14" s="1" t="s">
@@ -1198,13 +1198,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K15"/>
+      <c r="L15"/>
       <c r="M15" s="2" t="e">
-        <f>J15*L15</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N15" s="2" t="e">
-        <f>(I15-H15)*J15</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1234,13 +1234,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K16"/>
+      <c r="L16"/>
       <c r="M16" s="2" t="e">
-        <f>J16*L16</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N16" s="2" t="e">
-        <f>(I16-H16)*J16</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -1276,13 +1276,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K17"/>
+      <c r="L17"/>
       <c r="M17" s="2" t="e">
-        <f>J17*L17</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N17" s="2" t="e">
-        <f>(I17-H17)*J17</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1312,13 +1312,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K18"/>
+      <c r="L18"/>
       <c r="M18" s="2" t="e">
-        <f>J18*L18</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="2" t="e">
-        <f>(I18-H18)*J18</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1348,13 +1348,13 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K19"/>
+      <c r="L19"/>
       <c r="M19" s="2" t="e">
-        <f>J19*L19</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N19" s="2" t="e">
-        <f>(I19-H19)*J19</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added in try/except for reading files
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -425,8 +425,8 @@
     <col width="24.77734375" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
     <col width="7.21875" bestFit="1" customWidth="1" style="1" min="15" max="15"/>
     <col width="52.21875" bestFit="1" customWidth="1" style="9" min="16" max="16"/>
-    <col width="20.44140625" customWidth="1" style="1" min="17" max="18"/>
-    <col width="20.44140625" customWidth="1" style="1" min="19" max="16384"/>
+    <col width="20.44140625" customWidth="1" style="1" min="17" max="23"/>
+    <col width="20.44140625" customWidth="1" style="1" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
added check for currency CAD or USD only
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devra\Documents\Shakti Files\Projects\Scraping Stock Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFBED8E-D435-463C-B867-308A3D4B76F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ED69AD-9F30-41FE-86F1-4042EC385D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,8 +704,8 @@
     <col min="14" max="14" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="52.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="20.44140625" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="20.44140625" style="1"/>
+    <col min="17" max="18" width="20.44140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="20.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ticker column in Excel is used to iterate over sheets
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devra\Documents\Shakti Files\Projects\Scraping Stock Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ED69AD-9F30-41FE-86F1-4042EC385D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E533E35-6D3A-42B6-B55E-0B74F85577D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Potential_Investments" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Potential_Investments!$A$1:$N$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Potential_Investments!$B$1:$N$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -683,13 +683,13 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -710,10 +710,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -860,10 +860,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -1151,10 +1151,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>60</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1442,10 +1442,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>60</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -1635,8 +1635,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N18" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N19">
+  <autoFilter ref="B1:N18" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N19">
       <sortCondition descending="1" ref="N1:N18"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
switched main file to Stock_Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Stock_Analysis.xlsx
+++ b/Stock_Analysis.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devra\Documents\Shakti Files\Projects\Scraping Stock Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E533E35-6D3A-42B6-B55E-0B74F85577D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A212E-FF22-4C47-98B7-6B952F13CF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Potential_Investments" sheetId="1" r:id="rId1"/>
+    <sheet name="Personal_Investments" sheetId="2" r:id="rId2"/>
+    <sheet name="Current_Holdings" sheetId="3" r:id="rId3"/>
+    <sheet name="Account_Summary" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Potential_Investments!$B$1:$N$18</definedName>
   </definedNames>
@@ -33,14 +39,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="109">
+  <si>
+    <t>Ticker</t>
+  </si>
   <si>
     <t>Stock Name</t>
   </si>
   <si>
-    <t>Ticker</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -119,36 +125,36 @@
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=ZEB</t>
   </si>
   <si>
+    <t>CWB</t>
+  </si>
+  <si>
     <t>Canadian Western Bank</t>
   </si>
   <si>
-    <t>CWB</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=CWB</t>
   </si>
   <si>
+    <t>CTC.A</t>
+  </si>
+  <si>
     <t>Canadian Tire</t>
   </si>
   <si>
-    <t>CTC.A</t>
-  </si>
-  <si>
     <t>Goods</t>
   </si>
   <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=CTC.A</t>
   </si>
   <si>
+    <t>MFC</t>
+  </si>
+  <si>
     <t>Manulife</t>
   </si>
   <si>
-    <t>MFC</t>
-  </si>
-  <si>
     <t>Financial</t>
   </si>
   <si>
@@ -164,12 +170,12 @@
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=VEE</t>
   </si>
   <si>
+    <t>CM</t>
+  </si>
+  <si>
     <t>CIBC</t>
   </si>
   <si>
-    <t>CM</t>
-  </si>
-  <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=CM</t>
   </si>
   <si>
@@ -179,42 +185,42 @@
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=TD</t>
   </si>
   <si>
+    <t>RY</t>
+  </si>
+  <si>
     <t>RBC</t>
   </si>
   <si>
-    <t>RY</t>
-  </si>
-  <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=RY</t>
   </si>
   <si>
+    <t>ENB</t>
+  </si>
+  <si>
     <t>Enbridge</t>
   </si>
   <si>
-    <t>ENB</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=ENB</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>National Bank</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=NA</t>
   </si>
   <si>
+    <t>NFLX</t>
+  </si>
+  <si>
     <t>Netflix</t>
   </si>
   <si>
-    <t>NFLX</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -236,24 +242,24 @@
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=XUU</t>
   </si>
   <si>
+    <t>ZCN</t>
+  </si>
+  <si>
     <t>ZCN.TO</t>
   </si>
   <si>
-    <t>ZCN</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=ZCN</t>
   </si>
   <si>
+    <t>MSFT</t>
+  </si>
+  <si>
     <t>Microsoft</t>
   </si>
   <si>
-    <t>MSFT</t>
-  </si>
-  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -269,30 +275,106 @@
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=XEQT</t>
   </si>
   <si>
+    <t>CSU</t>
+  </si>
+  <si>
     <t>Constellation Software</t>
   </si>
   <si>
-    <t>CSU</t>
-  </si>
-  <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=CSU</t>
   </si>
   <si>
+    <t>L</t>
+  </si>
+  <si>
     <t>Loblaw</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>https://web.tmxmoney.com/quote.php?qm_symbol=L</t>
+  </si>
+  <si>
+    <t>Payment_Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Buy_Price</t>
+  </si>
+  <si>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy Value </t>
+  </si>
+  <si>
+    <t>Current_Value</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>Semi-Annual</t>
+  </si>
+  <si>
+    <t>https://web.tmxmoney.com/quote.php?qm_symbol=DIS:us</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>https://web.tmxmoney.com/quote.php?qm_symbol=GOOG:us</t>
+  </si>
+  <si>
+    <t>https://web.tmxmoney.com/quote.php?qm_symbol=N</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>https://web.tmxmoney.com/quote.php?qm_symbol=NVDA:us</t>
+  </si>
+  <si>
+    <t>TWTR</t>
+  </si>
+  <si>
+    <t>https://web.tmxmoney.com/quote.php?qm_symbol=TWTR:us</t>
+  </si>
+  <si>
+    <t>Total_Investments</t>
+  </si>
+  <si>
+    <t>CAD_Value</t>
+  </si>
+  <si>
+    <t>USD_Value</t>
+  </si>
+  <si>
+    <t>CAD_Profit</t>
+  </si>
+  <si>
+    <t>USD_Pofit</t>
+  </si>
+  <si>
+    <t>Exchange_Rate</t>
+  </si>
+  <si>
+    <t>Account_Val</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -337,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -366,11 +448,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -381,6 +509,147 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Potential_Investments"/>
+      <sheetName val="Personal_Investments"/>
+      <sheetName val="Current_Holdings"/>
+      <sheetName val="Account_Summary"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Currency</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>Current_Value</v>
+          </cell>
+          <cell r="L1" t="str">
+            <v>Profit</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K2">
+            <v>2958</v>
+          </cell>
+          <cell r="L2">
+            <v>-102</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K3">
+            <v>2830.8</v>
+          </cell>
+          <cell r="L3">
+            <v>-96.7199999999998</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>USD</v>
+          </cell>
+          <cell r="K4">
+            <v>1568.98</v>
+          </cell>
+          <cell r="L4">
+            <v>-265.02</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>USD</v>
+          </cell>
+          <cell r="K5">
+            <v>2863.94</v>
+          </cell>
+          <cell r="L5">
+            <v>633.72000000000025</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K6">
+            <v>148</v>
+          </cell>
+          <cell r="L6">
+            <v>-100</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>USD</v>
+          </cell>
+          <cell r="K7">
+            <v>1847.1000000000001</v>
+          </cell>
+          <cell r="L7">
+            <v>808.10000000000014</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>USD</v>
+          </cell>
+          <cell r="K8">
+            <v>507.68</v>
+          </cell>
+          <cell r="L8">
+            <v>-191.32480000000004</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K9">
+            <v>60.84</v>
+          </cell>
+          <cell r="L9">
+            <v>-0.77999999999999403</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K10">
+            <v>1411</v>
+          </cell>
+          <cell r="L10">
+            <v>-203.31999999999994</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="K11">
+            <v>1968</v>
+          </cell>
+          <cell r="L11">
+            <v>-32.799999999999955</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -682,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,16 +973,16 @@
     <col min="14" max="14" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="52.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="20.44140625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="20.44140625" style="1"/>
+    <col min="17" max="19" width="20.44140625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="20.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -778,7 +1047,7 @@
         <v>1000</v>
       </c>
       <c r="H2" s="7">
-        <v>75.989999999999995</v>
+        <v>73.95</v>
       </c>
       <c r="I2" s="1">
         <v>95</v>
@@ -799,7 +1068,7 @@
       </c>
       <c r="N2" s="2">
         <f t="shared" ref="N2:N19" si="2">(I2-H2)*J2</f>
-        <v>247.13000000000005</v>
+        <v>273.64999999999998</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -828,7 +1097,7 @@
         <v>1000</v>
       </c>
       <c r="H3" s="7">
-        <v>24.36</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1">
         <v>30</v>
@@ -849,7 +1118,7 @@
       </c>
       <c r="N3" s="2">
         <f t="shared" si="2"/>
-        <v>231.24</v>
+        <v>246</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -860,10 +1129,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
@@ -878,14 +1147,14 @@
         <v>1000</v>
       </c>
       <c r="H4" s="7">
-        <v>24.42</v>
+        <v>23.85</v>
       </c>
       <c r="I4" s="1">
         <v>30</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -895,11 +1164,11 @@
       </c>
       <c r="M4" s="2">
         <f t="shared" si="1"/>
-        <v>11.6</v>
+        <v>11.889999999999999</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="2"/>
-        <v>223.19999999999993</v>
+        <v>252.14999999999995</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>30</v>
@@ -910,10 +1179,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -928,7 +1197,7 @@
         <v>1000</v>
       </c>
       <c r="H5" s="7">
-        <v>119.61</v>
+        <v>117.95</v>
       </c>
       <c r="I5" s="1">
         <v>142</v>
@@ -949,7 +1218,7 @@
       </c>
       <c r="N5" s="2">
         <f t="shared" si="2"/>
-        <v>179.12</v>
+        <v>192.39999999999998</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>30</v>
@@ -960,10 +1229,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -978,14 +1247,14 @@
         <v>1000</v>
       </c>
       <c r="H6" s="7">
-        <v>18.690000000000001</v>
+        <v>18.2</v>
       </c>
       <c r="I6" s="1">
         <v>22</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -995,11 +1264,11 @@
       </c>
       <c r="M6" s="2">
         <f t="shared" si="1"/>
-        <v>14.840000000000002</v>
+        <v>15.120000000000001</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="2"/>
-        <v>175.42999999999992</v>
+        <v>205.20000000000005</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>39</v>
@@ -1028,7 +1297,7 @@
         <v>0.24</v>
       </c>
       <c r="H7" s="7">
-        <v>32.549999999999997</v>
+        <v>32.65</v>
       </c>
       <c r="I7" s="1">
         <v>36</v>
@@ -1049,7 +1318,7 @@
       </c>
       <c r="N7" s="2">
         <f t="shared" si="2"/>
-        <v>103.50000000000009</v>
+        <v>100.50000000000004</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>42</v>
@@ -1057,10 +1326,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -1075,7 +1344,7 @@
         <v>1000</v>
       </c>
       <c r="H8" s="7">
-        <v>93.49</v>
+        <v>92.64</v>
       </c>
       <c r="I8" s="1">
         <v>105</v>
@@ -1096,7 +1365,7 @@
       </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
-        <v>115.10000000000005</v>
+        <v>123.6</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>45</v>
@@ -1122,7 +1391,7 @@
         <v>1000</v>
       </c>
       <c r="H9" s="7">
-        <v>61.57</v>
+        <v>60.29</v>
       </c>
       <c r="I9" s="1">
         <v>69</v>
@@ -1143,7 +1412,7 @@
       </c>
       <c r="N9" s="2">
         <f t="shared" si="2"/>
-        <v>118.88</v>
+        <v>139.36000000000001</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>47</v>
@@ -1151,10 +1420,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -1169,7 +1438,7 @@
         <v>1000</v>
       </c>
       <c r="H10" s="7">
-        <v>92.36</v>
+        <v>91.71</v>
       </c>
       <c r="I10" s="1">
         <v>100</v>
@@ -1190,7 +1459,7 @@
       </c>
       <c r="N10" s="2">
         <f t="shared" si="2"/>
-        <v>76.400000000000006</v>
+        <v>82.900000000000063</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>50</v>
@@ -1198,10 +1467,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -1216,14 +1485,14 @@
         <v>1000</v>
       </c>
       <c r="H11" s="7">
-        <v>42.34</v>
+        <v>40.99</v>
       </c>
       <c r="I11" s="1">
         <v>45</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -1233,11 +1502,11 @@
       </c>
       <c r="M11" s="2">
         <f t="shared" si="1"/>
-        <v>18.630000000000003</v>
+        <v>19.440000000000001</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="2"/>
-        <v>61.179999999999922</v>
+        <v>96.239999999999952</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>54</v>
@@ -1245,10 +1514,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -1263,7 +1532,7 @@
         <v>1000</v>
       </c>
       <c r="H12" s="7">
-        <v>61.97</v>
+        <v>61.98</v>
       </c>
       <c r="I12" s="1">
         <v>65</v>
@@ -1284,7 +1553,7 @@
       </c>
       <c r="N12" s="2">
         <f t="shared" si="2"/>
-        <v>48.480000000000018</v>
+        <v>48.32000000000005</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>57</v>
@@ -1292,10 +1561,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>60</v>
@@ -1310,7 +1579,7 @@
         <v>1000</v>
       </c>
       <c r="H13" s="7">
-        <v>453.72</v>
+        <v>457.85</v>
       </c>
       <c r="I13" s="1">
         <v>450</v>
@@ -1331,7 +1600,7 @@
       </c>
       <c r="N13" s="2">
         <f t="shared" si="2"/>
-        <v>-7.4400000000000546</v>
+        <v>-15.700000000000045</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>63</v>
@@ -1360,14 +1629,14 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H14" s="7">
-        <v>31.67</v>
+        <v>31.02</v>
       </c>
       <c r="I14" s="1">
         <v>33</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -1377,11 +1646,11 @@
       </c>
       <c r="M14" s="2">
         <f t="shared" si="1"/>
-        <v>3.1929999999999996</v>
+        <v>3.2959999999999998</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="2"/>
-        <v>41.229999999999947</v>
+        <v>63.360000000000014</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -1392,10 +1661,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1413,14 +1682,14 @@
         <v>0.06</v>
       </c>
       <c r="H15" s="7">
-        <v>20.97</v>
+        <v>20.75</v>
       </c>
       <c r="I15" s="1">
         <v>22</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -1430,11 +1699,11 @@
       </c>
       <c r="M15" s="2">
         <f t="shared" si="1"/>
-        <v>8.93</v>
+        <v>9.120000000000001</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="2"/>
-        <v>48.410000000000053</v>
+        <v>60</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>70</v>
@@ -1442,10 +1711,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>60</v>
@@ -1460,7 +1729,7 @@
         <v>1000</v>
       </c>
       <c r="H16" s="7">
-        <v>195.15</v>
+        <v>197.84</v>
       </c>
       <c r="I16" s="1">
         <v>200</v>
@@ -1481,7 +1750,7 @@
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>24.249999999999972</v>
+        <v>10.799999999999983</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -1513,14 +1782,14 @@
         <v>0.2</v>
       </c>
       <c r="H17" s="7">
-        <v>20.65</v>
+        <v>20.28</v>
       </c>
       <c r="I17" s="1">
         <v>21.5</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -1530,11 +1799,11 @@
       </c>
       <c r="M17" s="2">
         <f t="shared" si="1"/>
-        <v>6.1920000000000002</v>
+        <v>6.3209999999999997</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="2"/>
-        <v>40.800000000000068</v>
+        <v>59.779999999999944</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>77</v>
@@ -1542,10 +1811,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -1560,14 +1829,14 @@
         <v>1000</v>
       </c>
       <c r="H18" s="7">
-        <v>471.8</v>
+        <v>1500</v>
       </c>
       <c r="I18" s="1">
         <v>500</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -1577,11 +1846,11 @@
       </c>
       <c r="M18" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="2"/>
-        <v>56.399999999999977</v>
+        <v>0</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>80</v>
@@ -1589,10 +1858,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -1607,14 +1876,14 @@
         <v>1000</v>
       </c>
       <c r="H19" s="7">
-        <v>67.150000000000006</v>
+        <v>66.13</v>
       </c>
       <c r="I19" s="1">
         <v>70</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -1624,11 +1893,11 @@
       </c>
       <c r="M19" s="2">
         <f t="shared" si="1"/>
-        <v>4.41</v>
+        <v>4.7249999999999996</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="2"/>
-        <v>39.89999999999992</v>
+        <v>58.050000000000068</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>83</v>
@@ -1643,4 +1912,683 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>43711</v>
+      </c>
+      <c r="B2" s="7">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>43805</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>43906</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>43917</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>43997</v>
+      </c>
+      <c r="B6" s="7">
+        <v>8000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7">
+        <v>40</v>
+      </c>
+      <c r="E2" s="14">
+        <v>76.5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>73.95</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="I2" s="14">
+        <f t="shared" ref="I2:I11" si="0">(D2*H2)</f>
+        <v>42.400000000000006</v>
+      </c>
+      <c r="J2" s="14">
+        <f t="shared" ref="J2:J11" si="1">(D2*E2)</f>
+        <v>3060</v>
+      </c>
+      <c r="K2" s="14">
+        <f t="shared" ref="K2:K11" si="2">D2*F2</f>
+        <v>2958</v>
+      </c>
+      <c r="L2" s="14">
+        <f t="shared" ref="L2:L11" si="3">K2-J2</f>
+        <v>-102</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
+        <v>24</v>
+      </c>
+      <c r="E3" s="14">
+        <v>121.98</v>
+      </c>
+      <c r="F3" s="7">
+        <v>117.95</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1.1375</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" si="0"/>
+        <v>27.299999999999997</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" si="1"/>
+        <v>2927.52</v>
+      </c>
+      <c r="K3" s="14">
+        <f t="shared" si="2"/>
+        <v>2830.8</v>
+      </c>
+      <c r="L3" s="14">
+        <f t="shared" si="3"/>
+        <v>-96.7199999999998</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7">
+        <v>14</v>
+      </c>
+      <c r="E4" s="14">
+        <v>131</v>
+      </c>
+      <c r="F4" s="7">
+        <v>112.07</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>12.32</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="1"/>
+        <v>1834</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="2"/>
+        <v>1568.98</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="3"/>
+        <v>-265.02</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1115.1099999999999</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1431.97</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="1"/>
+        <v>2230.2199999999998</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" si="2"/>
+        <v>2863.94</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="3"/>
+        <v>633.72000000000025</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>400</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.62</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.37</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="3"/>
+        <v>-100</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14">
+        <v>207.8</v>
+      </c>
+      <c r="F7" s="7">
+        <v>369.42</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="1"/>
+        <v>1039</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="2"/>
+        <v>1847.1000000000001</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="3"/>
+        <v>808.10000000000014</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7">
+        <v>16</v>
+      </c>
+      <c r="E8" s="14">
+        <v>43.687800000000003</v>
+      </c>
+      <c r="F8" s="7">
+        <v>31.73</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="1"/>
+        <v>699.00480000000005</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="2"/>
+        <v>507.68</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="3"/>
+        <v>-191.32480000000004</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14">
+        <v>20.54</v>
+      </c>
+      <c r="F9" s="7">
+        <v>20.28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.129</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="1"/>
+        <v>61.62</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="2"/>
+        <v>60.84</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="3"/>
+        <v>-0.77999999999999403</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7">
+        <v>68</v>
+      </c>
+      <c r="E10" s="14">
+        <v>23.74</v>
+      </c>
+      <c r="F10" s="7">
+        <v>20.75</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="0"/>
+        <v>12.92</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="1"/>
+        <v>1614.32</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="2"/>
+        <v>1411</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="3"/>
+        <v>-203.31999999999994</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7">
+        <v>82</v>
+      </c>
+      <c r="E11" s="14">
+        <v>24.4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>24</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="0"/>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="1"/>
+        <v>2000.8</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="2"/>
+        <v>1968</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="3"/>
+        <v>-32.799999999999955</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="L1:L11">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>0</formula>
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" style="14" customWidth="1"/>
+    <col min="4" max="5" width="10.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" s="14" t="e">
+        <f>SUMIF([1]Current_Holdings!B:B,"CAD",[1]Current_Holdings!K:K)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C2" s="14" t="e">
+        <f>SUMIF([1]Current_Holdings!B:B,"USD",[1]Current_Holdings!K:K)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D2" s="14" t="e">
+        <f>SUMIF([1]Current_Holdings!B:B, "CAD",[1]Current_Holdings!L:L)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E2" s="14" t="e">
+        <f>SUMIF([1]Current_Holdings!B:B, "USD",[1]Current_Holdings!L:L)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1.36</v>
+      </c>
+      <c r="G2" s="14" t="e">
+        <f>(C2*F2)+B2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>